<commit_message>
atualização do arquivo para python
</commit_message>
<xml_diff>
--- a/a3_euclerio.xlsx
+++ b/a3_euclerio.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,254 +451,254 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Valor final</t>
+          <t>Valor Final</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Aspirador Pó E Água 14l 1250w Power Lavor + Bico Extratora</t>
+          <t>Ar condicionado Philco  split inverter  frio 9000 BTU  branco 220V PAC9000IFM15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>379</t>
+          <t>2.529</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>299</t>
+          <t>1.897</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Casaco Masculino Jaqueta Puffer Bobojaco Corta Vento Frio Nf</t>
+          <t>Caixa De Som Partybox Stage 320 Jbl - Blpbstage320br</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>4.501</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>3.349</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cerveja Heineken Premium Garrafa 6 Long Neck 330ml</t>
+          <t>Console padrão Ps5 Slim Bundle Ratchet &amp; Clank and Returnal Cor Branco</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>4.399</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>3.899</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Coberdrom Casal Queen Size Cobertor Edredom Pele Carneiro</t>
+          <t>Cooktop 5 Bocas A Gás Dako Supreme Tripla Chama Preto Bivolt 110/220V</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>848</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>655</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Coberdrom Dupla Face Solteiro Sherpa Pele De Carneiro Big</t>
+          <t>Cooktop Itatiaia Essencial 4 Bocas - Preto</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>439</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>385</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Console padrão Ps5 Slim Bundle Ratchet &amp; Clank and Returnal Cor Branco</t>
+          <t>Creatina Monohidratada 500g Soldiers Nutrition Sabor Natural</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4.332</t>
+          <t>139</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>3.704</t>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Cooktop Itatiaia 5 Bocas Essencial Preto - Bivolt 110V/220V</t>
+          <t>Creatina Monohidratada 600g 100% Pura Soldiers Nutrition</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>599</t>
+          <t>154</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>398</t>
+          <t>114</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Creatina Monohidratada 500g Soldiers Nutrition Sabor Natural</t>
+          <t>Fogão  de pé Atlas Atenas Glass  4Q  gás engarrafado 4 queimadores  preto 127V/220V porta com visor 50L</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>1.039</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>733</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Creatina Monohidratada 600g 100% Pura Soldiers Nutrition</t>
+          <t>Fogão Atlas 4 Bocas Preto Atenas Glass - Bivolt</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>1.039</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>733</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Câmera de Vídeo Inteligente Wi-Fi Full HD iM3 C Black Intelbras</t>
+          <t>Forno Elétrico Philco Pfe44p Dupla Resistência 44l Cor Preto 110V</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>329</t>
+          <t>439</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>229</t>
+          <t>349</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Edredom Sherpa Cobertor E Coberdrom Casal Queen Grosso Cores</t>
+          <t>Fralda Pampers Pants Ajuste Total Max Xxg 78 Unidades</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>213</t>
+          <t>154</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>103</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Escova Secadora Bec07r Soft 4 Em 1 1300w Britânia Bivolt</t>
+          <t>Impressora Multifuncional 3 Em 1 Ecotank L3250 Preta Epson Cor Preto Bivolt</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>199</t>
+          <t>1.195</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>111</t>
+          <t>1.079</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Fritadeira Elétrica Mondial  AFO-12L-BI Forno Oven 12L Cor Preto/Inox 110V</t>
+          <t>Impressora a cor multifuncional Epson EcoTank L3250 com wifi preta 220V</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -707,769 +707,709 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>721</t>
+          <t>989</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Impressora Multifuncional 3 Em 1 Ecotank L3250 Preta Epson Cor Preto Bivolt</t>
+          <t>Mercado Pago: Point Pro2 - A Maquininha De Cartão + Completa</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1.195</t>
+          <t>149</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1.079</t>
+          <t>118</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Jogo De Lençol Queen 3 Peças 400 Fios C/ Elástico Hotel</t>
+          <t>Micro-ondas Efficient 23 Litros Me23b Branco Electrolux 110v</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>799</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>554</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Kit 10 Cuecas Box Boxer Estampadas Masculino Atacado Revenda</t>
+          <t>Micro-ondas Electrolux de bancada Branco com Função Tira Odor e Manter Aquecido 34L MEO44 127v</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>799</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>677</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Kit 10 Cuecas Masculinas Boxer Microfibra Polo Wear Sortido</t>
+          <t>Micro-ondas Philco Pmo23e 20l Espelhado 1100w Tira Odor 110v 127V</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>199</t>
+          <t>799</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>599</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Kit 2 Câmera Ip Wifi Dome Rotativa Visão Noturna A8 Cor Branco</t>
+          <t>Modulo Taramps Ts400x4 400w 2 Ohms Rca Ts 400x4 4 Canais 100w Amplificador 400rms T400 4 Canais Potencia Taramps Som Para Carro Moto Caminhonete Automotivo</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>222</t>
+          <t>221</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>197</t>
+          <t>187</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Kit Com 10 Cuecas Slip Go Tagless Masculina Zorba</t>
+          <t>Monitor Gamer Samsung T350 24” FHD, Tela Plana, 75Hz, 5ms, HDMI, FreeSync, Game Mode</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>729</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>653</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Lavadora De Alta Pressão 1500w 1750psi Wap Ousada Plus 2200 110V</t>
+          <t>Motorola Moto G24 128GB Grafite 8GB RAM</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>661</t>
+          <t>1.099</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>489</t>
+          <t>819</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Mercado Pago: Máquina De Cartão Point Smart 2 4g Wifi</t>
+          <t>Motorola Moto G24 128GB Rosa 8GB RAM</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>349</t>
+          <t>999</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>269</t>
+          <t>747</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Mercado Pago: Point Pro2 - A Maquininha De Cartão + Completa</t>
+          <t>Motorola Moto G24 128GB Verde 8GB RAM</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>999</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>129</t>
+          <t>747</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Micro-ondas Efficient 23 Litros Me23b Branco Electrolux 110v</t>
+          <t>Motorola Moto G54 5G 256 GB Azul 8 GB RAM</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>799</t>
+          <t>1.799</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>549</t>
+          <t>1.169</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Micro-ondas Efficient 23 Litros Me23b Branco Electrolux 220v</t>
+          <t>Notebook Acer Asp3 A315-510p-34xc I3 8gb 256gb Ssd 15.6 W11</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>659</t>
+          <t>3.799</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>549</t>
+          <t>2.338</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Micro-ondas Electrolux 34 Litros Meo44 220V</t>
+          <t>Notebook Acer Aspire 5 A515-57-55b8 Intel Core I5 8gb 256gb SSD 15,6'' W11</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>799</t>
+          <t>4.331</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>649</t>
+          <t>2.789</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Microondas Electrolux 31 Litros Capacidade Prata Mi41s 110V</t>
+          <t>Notebook Lenovo Ideapad Celeron 4gb 128ssd 15.6 W11 C/office Cor Cinza</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>999</t>
+          <t>2.665</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>829</t>
+          <t>1.799</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Mondial  Cozinha 4675-02 AFN-40-BFT Preto 110V</t>
+          <t>Notebook Samsung Galaxy Book2 I5-1235u Windows 11 Home 8gb 256gb Ssd Grafite</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>569</t>
+          <t>4.665</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>2.899</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Motorola Moto G04 128GB Grafite 4GB RAM</t>
+          <t>Paco Rabanne One million 1 Million Tradicional EDT 200ml para masculino</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>849</t>
+          <t>848</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>739</t>
+          <t>548</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Motorola Moto G24 128GB Grafite 8GB RAM</t>
+          <t>Parafusadeira E Furadeira Wap Impacto 21v 3/8 K21 Id02 Nova Cor Amarelo Frequência 50/60 Hz 110V/220V</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>999</t>
+          <t>348</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>724</t>
+          <t>279</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Motorola Moto G24 128GB Rosa 8GB RAM</t>
+          <t>Parafusadeira Furadeira De Impacto Profissional 21v  Modelo TB-21PX 2 Baterias Com Maleta Tb21px The Black Tools</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>999</t>
+          <t>374</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>747</t>
+          <t>289</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Motorola Moto G54 5G 256 GB Azul 8 GB RAM</t>
+          <t>Parafusadeira Furadeira Sem Fio Bateria 12v P/ Madeira Metal Cor Amarelo/Preto Frequência 60 110V/220V</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1.799</t>
+          <t>210</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.169</t>
+          <t>159</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Máquina de Lavar 14kg Electrolux Essential Care Cesto Inox 127v</t>
+          <t>Philco  PMO23EB Branco 220V</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2.885</t>
+          <t>699</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.849</t>
+          <t>514</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Notebook Acer Asp3 A315-510p-34xc I3 8gb 256gb Ssd 15.6 W11</t>
+          <t>Samsung Galaxy A15 4G Dual SIM 128 GB Azul claro 4 GB RAM</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3.099</t>
+          <t>1.415</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2.250</t>
+          <t>889</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Notebook Acer Aspire 5 A515-57-55b8 Intel Core I5 8gb 256gb SSD 15,6'' W11</t>
+          <t>Samsung Galaxy A15 4G Dual SIM 128 GB Azul escuro 4 GB RAM</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2.979</t>
+          <t>1.415</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2.728</t>
+          <t>869</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Notebook Samsung Galaxy Book2 I5-1235u Windows 11 Home 8gb 256gb Ssd Grafite</t>
+          <t>Samsung Galaxy A15 Dual SIM 4G 256GB Azul claro 8GB RAM</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4.665</t>
+          <t>1.499</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2.899</t>
+          <t>1.079</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Parafusadeira E Furadeira Wap Impacto 21v 3/8 K21 Id02 Nova Cor Amarelo Frequência 50/60 Hz 110V/220V</t>
+          <t>Samsung Galaxy A15 Dual SIM 5G 256GB Azul-escuro 8GB RAM</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>348</t>
+          <t>1.799</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>279</t>
+          <t>1.259</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Parafusadeira Furadeira Sem Fio Bateria 12v P/ Madeira Metal Cor Amarelo/Preto Frequência 60 110V/220V</t>
+          <t>Samsung Galaxy Tab S9 Fe Wifi, 128gb, 6gb Ram, Tela 10.9 Cor Cinza</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>2.989</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>159</t>
+          <t>2.357</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Philco  PMO23EB Branco 220V</t>
+          <t>Samsung Smart Tv 43'' Uhd 4k 43cu7700 2023</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>699</t>
+          <t>3.402</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>499</t>
+          <t>1.984</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A15 4G Dual SIM 128 GB Azul claro 4 GB RAM</t>
+          <t>Smart TV LG 32’’ LED HD 32LQ621 Bivolt Preta - Experiência Visual Incrível</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>1.072</t>
+          <t>1.499</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>813</t>
+          <t>1.089</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A15 5G Tela de 6.5" 90Hz 256GB Dual Chip Azul Claro</t>
+          <t>Smart TV LG AI ThinQ 43LM631C0SB LED webOS Full HD 43" 100V/240V</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1.799</t>
+          <t>1.865</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.169</t>
+          <t>1.641</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Samsung Galaxy A25 5G Dual SIM 256GB Azul-escuro 8GB RAM</t>
+          <t>Smart Tv 43 4k Uhd Thinq Ai 43ur7800 Hdr 10 Pro LG Bivolt</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2.249</t>
+          <t>2.998</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.380</t>
+          <t>1.798</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Samsung Smart Tv 43'' Uhd 4k 43cu7700 2023</t>
+          <t>Smart Tv 43'' Android Dolby Aws-tv-43-bl-02-a Aiwa Bivolt</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>3.402</t>
+          <t>1.899</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2.029</t>
+          <t>1.439</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Smart TV LG 32’’ LED HD 32LQ621 Bivolt Preta - Experiência Visual Incrível</t>
+          <t>Smart Tv LG 50 Led 4k Uhd Wi-fi Bluetooth  Hdr10 50ur871c0sa Preto</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>1.254</t>
+          <t>3.498</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.129</t>
+          <t>2.199</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Smart TV LG AI ThinQ 43LM631C0SB LED webOS Full HD 43" 100V/240V</t>
+          <t>Smart Tv Led 42'' Ptv42g6fr2cpf Roku Dolby Audio Preta Philco 110V/220V</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>1.750</t>
+          <t>1.823</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.540</t>
+          <t>1.459</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Smart Tv 43'' Android Dolby Aws-tv-43-bl-02-a Aiwa Bivolt</t>
+          <t>Smartphone Motorola Moto g04s 128GB 8GB Ram Boost Camera 16MP com Moto AI sensor FPS lateral - Grafite</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>1.899</t>
+          <t>879</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.439</t>
+          <t>699</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Smart Tv 43pfg6918/78 Full Hd 43'' Google Philips 110v/220v</t>
+          <t>Suplemento em Pó Max Titanium sem Sabor em Pote 3000mg</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>1.949</t>
+          <t>100</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.529</t>
+          <t>80</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Smart Tv LG 50 Led 4k Uhd Wi-fi Bluetooth  Hdr10 50ur871c0sa Preto</t>
+          <t>Tablet Samsung Galaxy Tab A9+ 5g 64gb 4gb Ram Grafite</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>3.498</t>
+          <t>1.499</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2.199</t>
+          <t>1.249</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Smart Tv Uhd 50UR8750PSA 50 Polegadas 4k 2023 LG Ashed Blue</t>
+          <t>Varal De Chão Grande Varal De Roupas 3 Andares Dobrável Cor Azul</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>3.739</t>
+          <t>120</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D49" t="inlineStr">
-        <is>
-          <t>2.243</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>Smartphone Motorola Moto g04s 128GB 8GB Ram Boost Camera 16MP com Moto AI sensor FPS lateral - Grafite</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>879</t>
-        </is>
-      </c>
-      <c r="C50" t="n">
-        <v>20</v>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>699</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>Tablet Samsung Galaxy Tab A9+ 5g 64gb 4gb Ram Grafite</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>1.499</t>
-        </is>
-      </c>
-      <c r="C51" t="n">
-        <v>16</v>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>1.249</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Varal De Chão Grande Varal De Roupas 3 Andares Dobrável Cor Azul</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="C52" t="n">
-        <v>18</v>
-      </c>
-      <c r="D52" t="inlineStr">
         <is>
           <t>97</t>
         </is>

</xml_diff>